<commit_message>
making figures on illustrator for manuscript submission; also added a couple tables for GO
</commit_message>
<xml_diff>
--- a/Data_Files/BP_GOterms_of_interest_sup.xlsx
+++ b/Data_Files/BP_GOterms_of_interest_sup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariaingersoll/Desktop/BU_Research/Davies-Gilmore/Aip_FS_2022/Aiptasia_Fed_Starved/Data_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7551C32-4844-0D48-8058-3FF70C5234FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C422C94A-0CE9-9147-B280-1BAE9D88CB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="1000" windowWidth="22800" windowHeight="15880" activeTab="1" xr2:uid="{BD502E35-1F59-A342-8A51-7D9BBB58FBF6}"/>
+    <workbookView xWindow="5620" yWindow="980" windowWidth="22800" windowHeight="15880" activeTab="1" xr2:uid="{BD502E35-1F59-A342-8A51-7D9BBB58FBF6}"/>
   </bookViews>
   <sheets>
     <sheet name="BPapo_aip" sheetId="2" r:id="rId1"/>
@@ -5680,7 +5680,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> oxidative stress/ROS response GO terms for DEG analysis (Fig. 3C)</a:t>
+            <a:t> oxidative stress/ROS response GO terms for DEG analysis (Fig. 3B)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200" b="1">
             <a:solidFill>
@@ -5864,7 +5864,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> oxidative stress/ROS response GO terms for DEG analysis (Fig. 3C)</a:t>
+            <a:t> oxidative stress/ROS response GO terms for DEG analysis (Fig. 3B)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200" b="1">
             <a:solidFill>
@@ -6266,7 +6266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB59ED7-CA34-9047-BF89-4E8DEFE7093C}">
   <dimension ref="A1:I796"/>
   <sheetViews>
-    <sheetView topLeftCell="A664" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -24597,8 +24597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C4129-D8D0-514A-B02D-EDC82AC40219}">
   <dimension ref="A1:G484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>